<commit_message>
Timing Results for BCGS
</commit_message>
<xml_diff>
--- a/results/2D_Results/R2/Timing_results.xlsx
+++ b/results/2D_Results/R2/Timing_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="full_hypre (2)" sheetId="1" state="visible" r:id="rId2"/>
@@ -184,23 +184,23 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.5"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,18 +504,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.6185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,11 +843,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="11" min="4" style="1" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="4" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,6 +889,14 @@
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -897,6 +905,14 @@
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -904,6 +920,33 @@
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1.7253507721289E-010</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.00023017137239509</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.2214224821</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>2.696783343</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>446.9183317123</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>449.6151316394</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>47.3735166304</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>47.3735270082</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,6 +956,33 @@
       <c r="B5" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>9.506452256118E-011</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.00023017137260259</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.1196586295</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>1.5033511788</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>181.5855268028</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>183.0888965869</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>26.7883942205</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>26.7884045252</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -920,6 +990,33 @@
       </c>
       <c r="B6" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4.1202575554487E-010</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.00023017137259984</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.0616104063</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>0.7892406357</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>54.2893862175</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>55.0786460205</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>14.1369411747</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>14.1369528537</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,6 +1026,33 @@
       <c r="B7" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>2.1046551056235E-010</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.0002301713723063</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.0325132696</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0.4025836837</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>16.1595630834</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>16.5621819183</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>7.8431197993</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>7.843144716</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -936,6 +1060,33 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>64</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>4.8162963120024E-010</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.00023017137249261</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.0190281091</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.2109954786</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>5.1019151299</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>5.3129964661</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>5.6299329695</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>5.6299969828</v>
       </c>
     </row>
   </sheetData>
@@ -962,11 +1113,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="12" min="4" style="1" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="12" min="4" style="1" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1078,17 +1229,17 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="11" min="4" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="11" min="4" style="1" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,6 +1313,33 @@
       <c r="B6" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4.0835231674808E-010</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>5.7477243126367E-005</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.2474672632</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>3.1432230861</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>758.8059399162</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>761.9491857614</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>59.6765665637</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>59.6765805297</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1170,6 +1348,33 @@
       <c r="B7" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4.4031378066206E-010</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>5.7477243317198E-005</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.1324929758</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>1.6267713022</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>223.1720150415</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>224.7988406424</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>42.2347568727</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>42.2347812589</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1177,6 +1382,33 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>64</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>1.4853340375077E-009</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>5.7477243111602E-005</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.0689320307</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0.9686685738</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>63.1584382067</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>64.1272050631</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>21.7812048834</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>21.7812723746</v>
       </c>
     </row>
   </sheetData>
@@ -1203,13 +1435,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.25555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.78148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.0074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="7" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.35185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.88148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.6925925925926"/>
+    <col collapsed="false" hidden="false" max="12" min="7" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>